<commit_message>
Upadte Home Budget Document
</commit_message>
<xml_diff>
--- a/Budget_Home.xlsx
+++ b/Budget_Home.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Docs_Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF1778CB-5AB5-4018-96F2-14A493A50904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6686E5E-B81D-453A-B4DE-26591248E0CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="820" firstSheet="13" activeTab="15" xr2:uid="{501F6562-0567-4B1B-9862-921E6A7B9365}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="820" firstSheet="13" activeTab="16" xr2:uid="{501F6562-0567-4B1B-9862-921E6A7B9365}"/>
   </bookViews>
   <sheets>
     <sheet name="LIC Details" sheetId="4" r:id="rId1"/>
@@ -415,7 +415,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="342">
   <si>
     <t>Value Date</t>
   </si>
@@ -1504,9 +1504,6 @@
     <t>Paid 31st March '21</t>
   </si>
   <si>
-    <t>Paid Immediately in March '21</t>
-  </si>
-  <si>
     <t>Paid Immediately in 1st April '21</t>
   </si>
   <si>
@@ -1558,13 +1555,36 @@
     <t>LIC Loan</t>
   </si>
   <si>
-    <t>Salary + Variable + LTA</t>
-  </si>
-  <si>
     <t>Disbursement in Bank</t>
   </si>
   <si>
     <t>RD Maturity</t>
+  </si>
+  <si>
+    <t>April '21</t>
+  </si>
+  <si>
+    <t>Salary + Variable</t>
+  </si>
+  <si>
+    <t>Pay From</t>
+  </si>
+  <si>
+    <t>FD</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>PAID</t>
+  </si>
+  <si>
+    <t>Paid Immediately in March '21
+Policy#903569252</t>
+  </si>
+  <si>
+    <t>Paid Immediately in March '21
+Policy#903569253</t>
   </si>
 </sst>
 </file>
@@ -1947,7 +1967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="232">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2409,11 +2429,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2465,24 +2500,35 @@
     <xf numFmtId="16" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3411,96 +3457,96 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="196">
+      <c r="A9" s="205">
         <v>3</v>
       </c>
-      <c r="B9" s="198" t="s">
+      <c r="B9" s="207" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="198" t="s">
+      <c r="C9" s="207" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="200"/>
+      <c r="D9" s="209"/>
       <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="202">
+      <c r="F9" s="211">
         <v>5800</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="197"/>
-      <c r="B10" s="199"/>
-      <c r="C10" s="199"/>
-      <c r="D10" s="201"/>
+      <c r="A10" s="206"/>
+      <c r="B10" s="208"/>
+      <c r="C10" s="208"/>
+      <c r="D10" s="210"/>
       <c r="E10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="203"/>
+      <c r="F10" s="212"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="196">
+      <c r="A11" s="205">
         <v>15</v>
       </c>
-      <c r="B11" s="198" t="s">
+      <c r="B11" s="207" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="198" t="s">
+      <c r="C11" s="207" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="200"/>
+      <c r="D11" s="209"/>
       <c r="E11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="202">
+      <c r="F11" s="211">
         <v>5800</v>
       </c>
-      <c r="G11" s="204"/>
-      <c r="H11" s="202"/>
+      <c r="G11" s="213"/>
+      <c r="H11" s="211"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="197"/>
-      <c r="B12" s="199"/>
-      <c r="C12" s="199"/>
-      <c r="D12" s="201"/>
+      <c r="A12" s="206"/>
+      <c r="B12" s="208"/>
+      <c r="C12" s="208"/>
+      <c r="D12" s="210"/>
       <c r="E12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="203"/>
-      <c r="G12" s="205"/>
-      <c r="H12" s="203"/>
+      <c r="F12" s="212"/>
+      <c r="G12" s="214"/>
+      <c r="H12" s="212"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="196">
+      <c r="A13" s="205">
         <v>16</v>
       </c>
-      <c r="B13" s="198" t="s">
+      <c r="B13" s="207" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="198" t="s">
+      <c r="C13" s="207" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="200"/>
+      <c r="D13" s="209"/>
       <c r="E13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="202">
+      <c r="F13" s="211">
         <v>5800</v>
       </c>
-      <c r="G13" s="204"/>
-      <c r="H13" s="202"/>
+      <c r="G13" s="213"/>
+      <c r="H13" s="211"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="197"/>
-      <c r="B14" s="199"/>
-      <c r="C14" s="199"/>
-      <c r="D14" s="201"/>
+      <c r="A14" s="206"/>
+      <c r="B14" s="208"/>
+      <c r="C14" s="208"/>
+      <c r="D14" s="210"/>
       <c r="E14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="203"/>
-      <c r="G14" s="205"/>
-      <c r="H14" s="203"/>
+      <c r="F14" s="212"/>
+      <c r="G14" s="214"/>
+      <c r="H14" s="212"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -3556,40 +3602,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="212">
+      <c r="A1" s="221">
         <v>44075</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="212"/>
-      <c r="H1" s="212"/>
-      <c r="I1" s="212"/>
-      <c r="J1" s="212"/>
-      <c r="K1" s="212"/>
-      <c r="L1" s="212"/>
-      <c r="M1" s="212"/>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
+      <c r="M1" s="221"/>
     </row>
     <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="219" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
       <c r="G2" s="114"/>
-      <c r="H2" s="211" t="s">
+      <c r="H2" s="220" t="s">
         <v>166</v>
       </c>
-      <c r="I2" s="211"/>
-      <c r="J2" s="211"/>
-      <c r="K2" s="211"/>
-      <c r="L2" s="211"/>
-      <c r="M2" s="211"/>
+      <c r="I2" s="220"/>
+      <c r="J2" s="220"/>
+      <c r="K2" s="220"/>
+      <c r="L2" s="220"/>
+      <c r="M2" s="220"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -4292,38 +4338,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="212">
+      <c r="A1" s="221">
         <v>44105</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="212"/>
-      <c r="H1" s="212"/>
-      <c r="I1" s="212"/>
-      <c r="J1" s="212"/>
-      <c r="K1" s="212"/>
-      <c r="L1" s="212"/>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="219" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
       <c r="F2" s="114"/>
-      <c r="G2" s="211" t="s">
+      <c r="G2" s="220" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="211"/>
-      <c r="I2" s="211"/>
-      <c r="J2" s="211"/>
-      <c r="K2" s="211"/>
-      <c r="L2" s="211"/>
+      <c r="H2" s="220"/>
+      <c r="I2" s="220"/>
+      <c r="J2" s="220"/>
+      <c r="K2" s="220"/>
+      <c r="L2" s="220"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -4984,38 +5030,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="212">
+      <c r="A1" s="221">
         <v>44136</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="212"/>
-      <c r="H1" s="212"/>
-      <c r="I1" s="212"/>
-      <c r="J1" s="212"/>
-      <c r="K1" s="212"/>
-      <c r="L1" s="212"/>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="219" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
       <c r="F2" s="114"/>
-      <c r="G2" s="211" t="s">
+      <c r="G2" s="220" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="211"/>
-      <c r="I2" s="211"/>
-      <c r="J2" s="211"/>
-      <c r="K2" s="211"/>
-      <c r="L2" s="211"/>
+      <c r="H2" s="220"/>
+      <c r="I2" s="220"/>
+      <c r="J2" s="220"/>
+      <c r="K2" s="220"/>
+      <c r="L2" s="220"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -5685,38 +5731,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="212">
+      <c r="A1" s="221">
         <v>44166</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="212"/>
-      <c r="H1" s="212"/>
-      <c r="I1" s="212"/>
-      <c r="J1" s="212"/>
-      <c r="K1" s="212"/>
-      <c r="L1" s="212"/>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="219" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
       <c r="F2" s="114"/>
-      <c r="G2" s="211" t="s">
+      <c r="G2" s="220" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="211"/>
-      <c r="I2" s="211"/>
-      <c r="J2" s="211"/>
-      <c r="K2" s="211"/>
-      <c r="L2" s="211"/>
+      <c r="H2" s="220"/>
+      <c r="I2" s="220"/>
+      <c r="J2" s="220"/>
+      <c r="K2" s="220"/>
+      <c r="L2" s="220"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -6386,38 +6432,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="212" t="s">
+      <c r="A1" s="221" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="212"/>
-      <c r="H1" s="212"/>
-      <c r="I1" s="212"/>
-      <c r="J1" s="212"/>
-      <c r="K1" s="212"/>
-      <c r="L1" s="212"/>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="219" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
       <c r="F2" s="114"/>
-      <c r="G2" s="211" t="s">
+      <c r="G2" s="220" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="211"/>
-      <c r="I2" s="211"/>
-      <c r="J2" s="211"/>
-      <c r="K2" s="211"/>
-      <c r="L2" s="211"/>
+      <c r="H2" s="220"/>
+      <c r="I2" s="220"/>
+      <c r="J2" s="220"/>
+      <c r="K2" s="220"/>
+      <c r="L2" s="220"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -7048,26 +7094,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="212">
+      <c r="A1" s="221">
         <v>44228</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="212"/>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="211" t="s">
+      <c r="B2" s="220" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="116"/>
@@ -7388,8 +7434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4588F5-B144-4712-A68D-0D54D3DA480D}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7405,26 +7451,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="212">
+      <c r="A1" s="221">
         <v>44256</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="212"/>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="211" t="s">
+      <c r="B2" s="220" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="116"/>
@@ -7735,8 +7781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF25BCD7-403F-4682-8C4D-9874D3ECF04E}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7750,31 +7796,31 @@
     <col min="7" max="7" width="24.7109375" style="111" customWidth="1"/>
     <col min="8" max="8" width="18" style="113" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="113"/>
+    <col min="10" max="10" width="18.42578125" style="113" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.5703125" style="113" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="212">
+      <c r="A1" s="221">
         <v>44287</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="212"/>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
     </row>
     <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="211" t="s">
+      <c r="B2" s="220" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="211"/>
-      <c r="D2" s="211"/>
-      <c r="E2" s="211"/>
-      <c r="F2" s="211"/>
-      <c r="G2" s="211"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="116"/>
@@ -7796,12 +7842,12 @@
       <c r="G3" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="I3" s="217" t="s">
+      <c r="I3" s="222" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="217"/>
-      <c r="K3" s="218" t="s">
-        <v>334</v>
+      <c r="J3" s="222"/>
+      <c r="K3" s="195" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -7821,11 +7867,11 @@
         <v>17</v>
       </c>
       <c r="G4" s="111" t="s">
-        <v>326</v>
-      </c>
-      <c r="H4" s="215"/>
+        <v>325</v>
+      </c>
+      <c r="H4" s="194"/>
       <c r="I4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J4" s="113">
         <v>299000</v>
@@ -7851,13 +7897,13 @@
         <v>17</v>
       </c>
       <c r="G5" s="111" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I5" t="s">
-        <v>333</v>
-      </c>
-      <c r="J5" s="219">
-        <v>132101</v>
+        <v>335</v>
+      </c>
+      <c r="J5" s="196">
+        <v>110000</v>
       </c>
       <c r="K5" s="113" t="s">
         <v>35</v>
@@ -7880,12 +7926,12 @@
         <v>17</v>
       </c>
       <c r="G6" s="119" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I6" s="41" t="s">
-        <v>335</v>
-      </c>
-      <c r="J6" s="219"/>
+        <v>333</v>
+      </c>
+      <c r="J6" s="196"/>
       <c r="K6" s="113" t="s">
         <v>38</v>
       </c>
@@ -7895,7 +7941,7 @@
         <v>800</v>
       </c>
       <c r="C7" s="118" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D7" s="169" t="s">
         <v>35</v>
@@ -7908,7 +7954,7 @@
       </c>
       <c r="J7" s="120">
         <f>SUM(J4:J6)</f>
-        <v>431101</v>
+        <v>409000</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7916,7 +7962,7 @@
         <v>2000</v>
       </c>
       <c r="C8" s="104" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>38</v>
@@ -7926,7 +7972,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="110" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7934,7 +7980,7 @@
         <v>10000</v>
       </c>
       <c r="C9" s="104" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G9" s="108"/>
       <c r="H9" s="104"/>
@@ -7956,9 +8002,18 @@
         <v>17</v>
       </c>
       <c r="G10" s="108" t="s">
-        <v>324</v>
-      </c>
-      <c r="H10" s="104"/>
+        <v>323</v>
+      </c>
+      <c r="H10" s="41">
+        <v>10000</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>309</v>
+      </c>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="162">
@@ -7974,37 +8029,57 @@
         <v>36</v>
       </c>
       <c r="G11" s="110" t="s">
-        <v>328</v>
-      </c>
-      <c r="H11" s="104"/>
+        <v>327</v>
+      </c>
+      <c r="H11" s="41">
+        <v>25000</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>278</v>
+      </c>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="82">
         <v>200000</v>
       </c>
       <c r="C12" s="104" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D12" s="143" t="s">
         <v>216</v>
       </c>
       <c r="E12" s="143" t="s">
+        <v>322</v>
+      </c>
+      <c r="F12" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="108" t="s">
         <v>323</v>
       </c>
-      <c r="F12" s="84" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="108" t="s">
-        <v>324</v>
-      </c>
-      <c r="H12" s="104"/>
+      <c r="H12" s="225">
+        <v>1900</v>
+      </c>
+      <c r="I12" s="225" t="s">
+        <v>312</v>
+      </c>
+      <c r="J12" s="225" t="s">
+        <v>314</v>
+      </c>
+      <c r="K12" s="41" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="82">
         <v>17400</v>
       </c>
       <c r="C13" s="104" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D13" s="143" t="s">
         <v>216</v>
@@ -8016,28 +8091,39 @@
         <v>17</v>
       </c>
       <c r="G13" s="108" t="s">
-        <v>324</v>
-      </c>
-      <c r="H13" s="104"/>
+        <v>323</v>
+      </c>
+      <c r="H13" s="225">
+        <v>2500</v>
+      </c>
+      <c r="I13" s="225" t="s">
+        <v>316</v>
+      </c>
+      <c r="J13" s="225" t="s">
+        <v>317</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="82">
         <v>25000</v>
       </c>
       <c r="C14" s="104" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D14" s="143" t="s">
         <v>216</v>
       </c>
       <c r="E14" s="143" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F14" s="84" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="108" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H14" s="104"/>
     </row>
@@ -8046,7 +8132,7 @@
         <v>2500</v>
       </c>
       <c r="C15" s="104" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>35</v>
@@ -8058,7 +8144,7 @@
         <v>17</v>
       </c>
       <c r="G15" s="108" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H15" s="104"/>
     </row>
@@ -8178,7 +8264,7 @@
         <v>17</v>
       </c>
       <c r="G24" s="108" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H24" s="104"/>
     </row>
@@ -8274,7 +8360,7 @@
     <row r="40" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="82">
         <f>J7</f>
-        <v>431101</v>
+        <v>409000</v>
       </c>
       <c r="C40" s="104" t="s">
         <v>66</v>
@@ -8296,7 +8382,7 @@
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="83">
         <f>B40-B39</f>
-        <v>72901</v>
+        <v>50800</v>
       </c>
       <c r="C41" s="104" t="s">
         <v>108</v>
@@ -8323,10 +8409,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95534229-9251-45A5-AA67-E5DCE3AB28B0}">
-  <dimension ref="A2:L17"/>
+  <dimension ref="A2:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8337,11 +8423,13 @@
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="41"/>
+    <col min="11" max="11" width="25.5703125" style="41" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.28515625" style="41" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" s="57" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="57" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="168" t="s">
         <v>303</v>
       </c>
@@ -8357,46 +8445,54 @@
       <c r="E2" s="192" t="s">
         <v>304</v>
       </c>
+      <c r="F2" s="229"/>
       <c r="G2" s="151" t="s">
         <v>302</v>
       </c>
       <c r="H2" s="151" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="169">
+      <c r="M2" s="200" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="168">
         <v>1</v>
       </c>
-      <c r="B3" s="188">
+      <c r="B3" s="197">
         <v>903569252</v>
       </c>
-      <c r="C3" s="189">
+      <c r="C3" s="198">
         <v>44277</v>
       </c>
-      <c r="D3" s="195">
+      <c r="D3" s="193">
         <v>65000</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>2000</v>
       </c>
-      <c r="G3" s="194" t="s">
+      <c r="F3" s="229"/>
+      <c r="G3" s="230" t="s">
         <v>305</v>
       </c>
-      <c r="H3" s="193">
+      <c r="H3" s="199">
         <v>44277</v>
       </c>
-      <c r="J3" s="38">
+      <c r="J3" s="225">
         <v>25000</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="225" t="s">
         <v>306</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="226" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="57" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="169">
         <v>2</v>
       </c>
@@ -8412,23 +8508,23 @@
       <c r="E4">
         <v>1045</v>
       </c>
-      <c r="F4" s="187">
-        <f>D3+D4</f>
-        <v>125000</v>
-      </c>
-      <c r="G4" s="194"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="231"/>
       <c r="H4" s="57"/>
-      <c r="J4" s="216">
+      <c r="J4" s="227">
         <v>18000</v>
       </c>
-      <c r="K4" s="216" t="s">
+      <c r="K4" s="227" t="s">
         <v>297</v>
       </c>
-      <c r="L4" s="216" t="s">
+      <c r="L4" s="227" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="57" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="169">
         <v>3</v>
       </c>
@@ -8444,19 +8540,22 @@
       <c r="E5">
         <v>906</v>
       </c>
-      <c r="G5" s="194"/>
+      <c r="G5" s="231"/>
       <c r="H5" s="57"/>
-      <c r="J5" s="38">
+      <c r="J5" s="225">
         <v>17400</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="225" t="s">
         <v>185</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="226" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="57" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="169">
         <v>4</v>
       </c>
@@ -8472,19 +8571,22 @@
       <c r="E6">
         <v>938</v>
       </c>
-      <c r="G6" s="194"/>
+      <c r="G6" s="231"/>
       <c r="H6" s="57"/>
-      <c r="J6" s="38">
+      <c r="J6" s="225">
         <v>67000</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="225" t="s">
         <v>307</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="228" t="s">
+        <v>340</v>
+      </c>
+      <c r="M6" s="57" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="169">
         <v>5</v>
       </c>
@@ -8504,19 +8606,22 @@
         <f>D5+D6+D7</f>
         <v>127000</v>
       </c>
-      <c r="G7" s="194"/>
+      <c r="G7" s="231"/>
       <c r="H7" s="57"/>
-      <c r="J7" s="38">
-        <v>200000</v>
-      </c>
-      <c r="K7" s="38" t="s">
-        <v>308</v>
-      </c>
-      <c r="L7" s="38" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J7" s="225">
+        <v>61000</v>
+      </c>
+      <c r="K7" s="225" t="s">
+        <v>307</v>
+      </c>
+      <c r="L7" s="228" t="s">
+        <v>341</v>
+      </c>
+      <c r="M7" s="57" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="169">
         <v>6</v>
       </c>
@@ -8532,16 +8637,22 @@
       <c r="E8">
         <v>749</v>
       </c>
-      <c r="G8" s="194"/>
+      <c r="G8" s="231"/>
       <c r="H8" s="57"/>
-      <c r="J8">
-        <v>10000</v>
-      </c>
-      <c r="K8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J8" s="225">
+        <v>200000</v>
+      </c>
+      <c r="K8" s="225" t="s">
+        <v>308</v>
+      </c>
+      <c r="L8" s="225" t="s">
+        <v>315</v>
+      </c>
+      <c r="M8" s="57" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="169">
         <v>7</v>
       </c>
@@ -8557,16 +8668,10 @@
       <c r="E9">
         <v>876</v>
       </c>
-      <c r="G9" s="194"/>
+      <c r="G9" s="231"/>
       <c r="H9" s="57"/>
-      <c r="J9">
-        <v>25000</v>
-      </c>
-      <c r="K9" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="169">
         <v>8</v>
       </c>
@@ -8586,62 +8691,69 @@
         <f>D8+D9+D10</f>
         <v>114000</v>
       </c>
-      <c r="G10" s="194"/>
+      <c r="G10" s="231"/>
       <c r="H10" s="57"/>
-      <c r="J10" s="38">
-        <v>1900</v>
-      </c>
-      <c r="K10" s="38" t="s">
-        <v>312</v>
-      </c>
-      <c r="L10" s="38" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="169">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="168">
         <v>9</v>
       </c>
-      <c r="J11" s="38">
-        <v>2500</v>
-      </c>
-      <c r="K11" s="38" t="s">
-        <v>317</v>
-      </c>
-      <c r="L11" s="38" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="201">
+        <v>903569253</v>
+      </c>
+      <c r="C11" s="202">
+        <v>44289</v>
+      </c>
+      <c r="D11" s="203">
+        <v>59000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="230" t="s">
+        <v>339</v>
+      </c>
+      <c r="H11" s="204">
+        <v>44290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="169">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="169">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F14" s="48"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D15" s="48">
         <f>SUM(D3:D13)</f>
-        <v>366000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>425000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D16" s="48">
-        <f>D15-67000</f>
-        <v>299000</v>
-      </c>
-      <c r="J16">
-        <f>SUM(J3:J11)</f>
-        <v>366800</v>
+        <f>D15-J16</f>
+        <v>36600</v>
+      </c>
+      <c r="J16" s="41">
+        <f>SUM(J3:J15)</f>
+        <v>388400</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="48"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -8890,12 +9002,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="206" t="s">
+      <c r="B1" s="215" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="206"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
       <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
@@ -9477,7 +9589,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C30"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9489,13 +9601,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="223" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="213"/>
-      <c r="C1" s="213"/>
-      <c r="D1" s="213"/>
-      <c r="E1" s="214"/>
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="224"/>
     </row>
     <row r="2" spans="1:6" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="137">
@@ -9639,7 +9751,12 @@
       <c r="C14">
         <v>75000</v>
       </c>
-      <c r="D14" s="84"/>
+      <c r="D14" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="65" t="s">
@@ -9648,7 +9765,12 @@
       <c r="C15">
         <v>125000</v>
       </c>
-      <c r="D15" s="84"/>
+      <c r="D15" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
@@ -9659,10 +9781,11 @@
         <f>SUM(C13:C15)</f>
         <v>250100</v>
       </c>
-      <c r="D16" s="125"/>
+      <c r="D16" s="125" t="s">
+        <v>17</v>
+      </c>
       <c r="E16" s="128">
-        <f>C16-C13</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="F16" s="129" t="s">
         <v>108</v>
@@ -9693,6 +9816,9 @@
       <c r="C19">
         <v>1750</v>
       </c>
+      <c r="D19" s="84" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="65" t="s">
@@ -9701,6 +9827,9 @@
       <c r="C20">
         <v>1750</v>
       </c>
+      <c r="D20" s="84" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="65" t="s">
@@ -9708,6 +9837,9 @@
       </c>
       <c r="C21">
         <v>1750</v>
+      </c>
+      <c r="D21" s="84" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -9774,6 +9906,9 @@
       <c r="C27">
         <v>6666.67</v>
       </c>
+      <c r="D27" s="84" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="65" t="s">
@@ -9782,6 +9917,9 @@
       <c r="C28">
         <v>6666.67</v>
       </c>
+      <c r="D28" s="84" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="65" t="s">
@@ -9790,6 +9928,9 @@
       <c r="C29">
         <v>6666.66</v>
       </c>
+      <c r="D29" s="84" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="65" t="s">
@@ -9797,6 +9938,9 @@
       </c>
       <c r="C30">
         <v>6666.66</v>
+      </c>
+      <c r="D30" s="84" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -9810,8 +9954,7 @@
       </c>
       <c r="D31" s="31"/>
       <c r="E31" s="128">
-        <f>C31-C25-C26</f>
-        <v>26666.660000000003</v>
+        <v>0</v>
       </c>
       <c r="F31" s="129" t="s">
         <v>108</v>
@@ -9823,7 +9966,7 @@
       </c>
       <c r="C33" s="131">
         <f>E9+E16+E22+E31</f>
-        <v>271666.66000000003</v>
+        <v>45000</v>
       </c>
     </row>
   </sheetData>
@@ -10195,12 +10338,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="206" t="s">
+      <c r="B1" s="215" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="206"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
       <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
@@ -10507,12 +10650,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="206" t="s">
+      <c r="B1" s="215" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="206"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
       <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
@@ -10932,12 +11075,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="206" t="s">
+      <c r="B1" s="215" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="206"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
       <c r="F1" s="3"/>
       <c r="G1" s="2"/>
       <c r="I1" s="5">
@@ -11256,14 +11399,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="207">
+      <c r="A1" s="216">
         <v>43952</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
       <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -11591,14 +11734,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="207">
+      <c r="A1" s="216">
         <v>43983</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
       <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -12074,40 +12217,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="207">
+      <c r="A1" s="216">
         <v>44013</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="207"/>
-      <c r="I1" s="207"/>
-      <c r="J1" s="207"/>
-      <c r="K1" s="207"/>
-      <c r="L1" s="207"/>
-      <c r="M1" s="207"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="216"/>
+      <c r="H1" s="216"/>
+      <c r="I1" s="216"/>
+      <c r="J1" s="216"/>
+      <c r="K1" s="216"/>
+      <c r="L1" s="216"/>
+      <c r="M1" s="216"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="208" t="s">
+      <c r="A2" s="217" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="208"/>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
       <c r="G2" s="88"/>
-      <c r="H2" s="209" t="s">
+      <c r="H2" s="218" t="s">
         <v>133</v>
       </c>
-      <c r="I2" s="209"/>
-      <c r="J2" s="209"/>
-      <c r="K2" s="209"/>
-      <c r="L2" s="209"/>
-      <c r="M2" s="209"/>
+      <c r="I2" s="218"/>
+      <c r="J2" s="218"/>
+      <c r="K2" s="218"/>
+      <c r="L2" s="218"/>
+      <c r="M2" s="218"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -12673,38 +12816,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="207">
+      <c r="A1" s="216">
         <v>44044</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="207"/>
-      <c r="I1" s="207"/>
-      <c r="J1" s="207"/>
-      <c r="K1" s="207"/>
-      <c r="L1" s="207"/>
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="216"/>
+      <c r="H1" s="216"/>
+      <c r="I1" s="216"/>
+      <c r="J1" s="216"/>
+      <c r="K1" s="216"/>
+      <c r="L1" s="216"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="219" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
       <c r="F2" s="88"/>
-      <c r="G2" s="211" t="s">
+      <c r="G2" s="220" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="211"/>
-      <c r="I2" s="211"/>
-      <c r="J2" s="211"/>
-      <c r="K2" s="211"/>
-      <c r="L2" s="211"/>
+      <c r="H2" s="220"/>
+      <c r="I2" s="220"/>
+      <c r="J2" s="220"/>
+      <c r="K2" s="220"/>
+      <c r="L2" s="220"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">

</xml_diff>

<commit_message>
Expenses Updated in Excel Sheet
</commit_message>
<xml_diff>
--- a/Budget_Home.xlsx
+++ b/Budget_Home.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Docs_Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE725BD6-E943-45BD-910E-CE29BFDC4720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130F5B3C-F647-4605-B38C-7F141C2BED9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="820" firstSheet="13" activeTab="16" xr2:uid="{501F6562-0567-4B1B-9862-921E6A7B9365}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="820" firstSheet="13" activeTab="17" xr2:uid="{501F6562-0567-4B1B-9862-921E6A7B9365}"/>
   </bookViews>
   <sheets>
     <sheet name="LIC Details" sheetId="4" r:id="rId1"/>
@@ -30,11 +30,12 @@
     <sheet name="Feb 21" sheetId="26" r:id="rId15"/>
     <sheet name="March 21" sheetId="25" r:id="rId16"/>
     <sheet name="April 21" sheetId="28" r:id="rId17"/>
-    <sheet name="LIC Loan_NEW" sheetId="27" r:id="rId18"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId19"/>
-    <sheet name="LIC_Policies_dues" sheetId="10" r:id="rId20"/>
-    <sheet name="LOAN_Records" sheetId="14" r:id="rId21"/>
-    <sheet name="Yearly Fixed Expenses" sheetId="15" r:id="rId22"/>
+    <sheet name="May 21" sheetId="29" r:id="rId18"/>
+    <sheet name="LIC Loan_NEW" sheetId="27" r:id="rId19"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId20"/>
+    <sheet name="LIC_Policies_dues" sheetId="10" r:id="rId21"/>
+    <sheet name="LOAN_Records" sheetId="14" r:id="rId22"/>
+    <sheet name="Yearly Fixed Expenses" sheetId="15" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'April 20'!$B$2:$G$2</definedName>
@@ -89,6 +90,27 @@
       </text>
     </comment>
     <comment ref="H7" authorId="1" shapeId="0" xr:uid="{2BF63EB9-D792-4B2E-80C3-A7A8D7C15443}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Yrly =          7000 * 1 year [ 84000  ]
+LIC =          3000 * 2 years [ 72000 ]
+LIC =          2000 * 3 years [ 72000 ]
+Prisha =     3000 * 5 years [ 180000 ]</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={7F17BA64-0441-4D64-B968-98E3C912D01F}</author>
+  </authors>
+  <commentList>
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{7F17BA64-0441-4D64-B968-98E3C912D01F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -415,7 +437,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="364">
   <si>
     <t>Value Date</t>
   </si>
@@ -1605,14 +1627,59 @@
     <t>Cash Paid</t>
   </si>
   <si>
-    <t>Transf. to another bank Accpunt</t>
+    <t>Papa Doctor follow up</t>
+  </si>
+  <si>
+    <t>Mummy X-Ray</t>
+  </si>
+  <si>
+    <t>Transf. to another bank Ac</t>
+  </si>
+  <si>
+    <t>Class Fees 1st Installment</t>
+  </si>
+  <si>
+    <t>Transf. via PhonePe Using Contact Number</t>
+  </si>
+  <si>
+    <t>PhonePe Scan</t>
+  </si>
+  <si>
+    <t>Mummy Report [ Nidhi ]</t>
+  </si>
+  <si>
+    <t>Papa Medicines</t>
+  </si>
+  <si>
+    <t>Daily Milk for Home</t>
+  </si>
+  <si>
+    <t>Uber Remaining Balance</t>
+  </si>
+  <si>
+    <t>Mummy X-Ray at Home</t>
+  </si>
+  <si>
+    <t>Cash Withrawal</t>
+  </si>
+  <si>
+    <t>Papa Reports [ Nakoda - Pulse ] + Doctor Follow Up</t>
+  </si>
+  <si>
+    <t>KTK Transf</t>
+  </si>
+  <si>
+    <t>LIC Yearly</t>
+  </si>
+  <si>
+    <t>Mummy Medicines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1778,6 +1845,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2922,13 +2995,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1095375</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2937,6 +3010,64 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62415E96-CDC3-41CD-BFAD-528365964891}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="3581400"/>
+          <a:ext cx="2638425" cy="542925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1095375</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62BF4CD9-C92D-46C7-B823-0ED00F91663B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3292,6 +3423,17 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment10.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B21" dT="2020-06-17T04:44:43.67" personId="{A40AD1FD-EE49-4CC6-BEFC-81CD31439168}" id="{7F17BA64-0441-4D64-B968-98E3C912D01F}">
+    <text>Yrly =          7000 * 1 year [ 84000  ]
+LIC =          3000 * 2 years [ 72000 ]
+LIC =          2000 * 3 years [ 72000 ]
+Prisha =     3000 * 5 years [ 180000 ]</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A6" dT="2020-06-17T04:44:43.67" personId="{A40AD1FD-EE49-4CC6-BEFC-81CD31439168}" id="{BD7E5772-A2A6-44D1-AC79-5F9083F4A2C4}">
@@ -7800,10 +7942,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF25BCD7-403F-4682-8C4D-9874D3ECF04E}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B30"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7811,8 +7953,8 @@
     <col min="1" max="1" width="1.85546875" style="117" customWidth="1"/>
     <col min="2" max="2" width="17" style="64" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" style="119" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="57" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="143" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="143" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="84" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="111" customWidth="1"/>
     <col min="8" max="8" width="18" style="113" bestFit="1" customWidth="1"/>
@@ -8234,15 +8376,15 @@
       </c>
       <c r="H18" s="104"/>
     </row>
-    <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="162">
-        <v>15000</v>
+        <v>15600</v>
       </c>
       <c r="C19" s="104" t="s">
         <v>345</v>
       </c>
       <c r="D19" s="143" t="s">
-        <v>216</v>
+        <v>67</v>
       </c>
       <c r="E19" s="143" t="s">
         <v>346</v>
@@ -8250,227 +8392,421 @@
       <c r="F19" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="111" t="s">
+      <c r="G19" s="110" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="162">
+        <v>300</v>
+      </c>
+      <c r="C20" s="119" t="s">
         <v>348</v>
       </c>
+      <c r="D20" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="143" t="s">
+        <v>347</v>
+      </c>
+      <c r="F20" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="110" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="162">
+        <v>1500</v>
+      </c>
+      <c r="C21" s="119" t="s">
+        <v>349</v>
+      </c>
+      <c r="D21" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="143" t="s">
+        <v>347</v>
+      </c>
+      <c r="F21" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="110" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="162">
+        <v>10000</v>
+      </c>
+      <c r="C22" s="119" t="s">
+        <v>351</v>
+      </c>
+      <c r="D22" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="110" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="82">
+        <f>950+1800</f>
+        <v>2750</v>
+      </c>
+      <c r="C23" s="119" t="s">
+        <v>354</v>
+      </c>
+      <c r="D23" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="110" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="104" t="s">
+      <c r="B24" s="82">
+        <v>1500</v>
+      </c>
+      <c r="C24" s="119" t="s">
+        <v>358</v>
+      </c>
+      <c r="D24" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="143" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="110" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="82">
+        <f>1600+300</f>
+        <v>1900</v>
+      </c>
+      <c r="C25" s="119" t="s">
+        <v>360</v>
+      </c>
+      <c r="D25" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="110" t="s">
+        <v>353</v>
+      </c>
+      <c r="H25" s="104"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="162"/>
+      <c r="C26" s="104" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="162"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="104"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="165">
-        <v>10000</v>
-      </c>
-      <c r="C26" s="118" t="s">
-        <v>288</v>
-      </c>
-      <c r="D26" s="107" t="s">
-        <v>216</v>
-      </c>
-      <c r="E26" s="107" t="s">
-        <v>144</v>
-      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
       <c r="G26" s="108"/>
       <c r="H26" s="104"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="165">
+      <c r="B27" s="82">
+        <f>500</f>
+        <v>500</v>
+      </c>
+      <c r="C27" s="119" t="s">
+        <v>355</v>
+      </c>
+      <c r="D27" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="110"/>
+      <c r="H27" s="104"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="82">
+        <v>3000</v>
+      </c>
+      <c r="C28" s="119" t="s">
+        <v>356</v>
+      </c>
+      <c r="D28" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="110"/>
+      <c r="H28" s="104"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="82">
+        <v>125</v>
+      </c>
+      <c r="C29" s="119" t="s">
+        <v>357</v>
+      </c>
+      <c r="D29" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="110"/>
+      <c r="H29" s="104"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="82">
+        <v>1000</v>
+      </c>
+      <c r="C30" s="119" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="143" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="110" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" s="104"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="82"/>
+      <c r="G31" s="110"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="82"/>
+      <c r="G32" s="110"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="82"/>
+      <c r="G33" s="110"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="82"/>
+      <c r="G34" s="110"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="82"/>
+      <c r="G35" s="110"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="82"/>
+      <c r="G36" s="110"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G37" s="110"/>
+      <c r="H37" s="104"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G38" s="110"/>
+      <c r="H38" s="104"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G39" s="110"/>
+      <c r="H39" s="104"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G40" s="110"/>
+      <c r="H40" s="104"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G41" s="110"/>
+      <c r="H41" s="104"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G42" s="110"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="165">
         <v>10000</v>
       </c>
-      <c r="C27" s="118" t="s">
+      <c r="C43" s="118" t="s">
+        <v>288</v>
+      </c>
+      <c r="D43" s="107" t="s">
+        <v>216</v>
+      </c>
+      <c r="E43" s="107" t="s">
+        <v>144</v>
+      </c>
+      <c r="G43" s="108"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="165">
+        <v>10000</v>
+      </c>
+      <c r="C44" s="118" t="s">
         <v>289</v>
       </c>
-      <c r="D27" s="169" t="s">
+      <c r="D44" s="169" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="169" t="s">
+      <c r="E44" s="169" t="s">
         <v>149</v>
       </c>
-      <c r="G27" s="108"/>
-      <c r="H27" s="104"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="165">
+      <c r="G44" s="108"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="165">
         <v>3500</v>
       </c>
-      <c r="C28" s="104" t="s">
+      <c r="C45" s="104" t="s">
         <v>290</v>
       </c>
-      <c r="D28" s="169" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="169" t="s">
+      <c r="D45" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="169" t="s">
         <v>216</v>
       </c>
-      <c r="F28" s="84" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="108"/>
-      <c r="H28" s="104"/>
-    </row>
-    <row r="29" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="166">
+      <c r="F45" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" s="108"/>
+    </row>
+    <row r="46" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="166">
         <v>15000</v>
       </c>
-      <c r="C29" s="104" t="s">
+      <c r="C46" s="104" t="s">
         <v>298</v>
       </c>
-      <c r="D29" s="143" t="s">
+      <c r="D46" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="143" t="s">
+      <c r="E46" s="143" t="s">
         <v>291</v>
       </c>
-      <c r="G29" s="108"/>
-      <c r="H29" s="104"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="166">
+      <c r="G46" s="108"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="166">
         <v>3500</v>
       </c>
-      <c r="C30" s="104" t="s">
+      <c r="C47" s="104" t="s">
         <v>191</v>
       </c>
-      <c r="D30" s="143" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="143" t="s">
+      <c r="D47" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="143" t="s">
         <v>191</v>
       </c>
-      <c r="F30" s="84" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="108" t="s">
+      <c r="F47" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" s="108" t="s">
         <v>324</v>
       </c>
-      <c r="H30" s="104"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="83"/>
-      <c r="C31" s="104"/>
-      <c r="D31" s="143"/>
-      <c r="E31" s="143"/>
-      <c r="G31" s="108"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="83"/>
-      <c r="C32" s="104"/>
-      <c r="D32" s="143"/>
-      <c r="E32" s="143"/>
-      <c r="G32" s="108"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="83"/>
-      <c r="C33" s="104"/>
-      <c r="D33" s="143"/>
-      <c r="E33" s="143"/>
-      <c r="G33" s="108"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="83"/>
-      <c r="C34" s="104"/>
-      <c r="D34" s="143"/>
-      <c r="E34" s="143"/>
-      <c r="G34" s="108"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="83"/>
-      <c r="C35" s="104"/>
-      <c r="D35" s="143"/>
-      <c r="E35" s="143"/>
-      <c r="G35" s="108"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="83"/>
-      <c r="C36" s="104"/>
-      <c r="D36" s="143"/>
-      <c r="E36" s="143"/>
-      <c r="G36" s="108"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="145"/>
-      <c r="C37" s="118"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="G37" s="108"/>
-      <c r="H37" s="104"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="145"/>
-      <c r="C38" s="118"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="G38" s="108"/>
-      <c r="H38" s="104"/>
-    </row>
-    <row r="39" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B39" s="82">
-        <f>SUM(B4:B37)</f>
-        <v>379650</v>
-      </c>
-      <c r="C39" s="104" t="s">
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="83"/>
+      <c r="C48" s="104"/>
+      <c r="G48" s="108"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="145"/>
+      <c r="C49" s="118"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="G49" s="108"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="145"/>
+      <c r="C50" s="118"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="G50" s="108"/>
+    </row>
+    <row r="51" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="82">
+        <f>SUM(B4:B49)</f>
+        <v>402825</v>
+      </c>
+      <c r="C51" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="172" t="s">
+      <c r="D51" s="172" t="s">
         <v>221</v>
       </c>
-      <c r="E39" s="158">
-        <f>SUM(B4:B25)</f>
-        <v>337650</v>
-      </c>
-      <c r="F39" s="84">
-        <f>E39*12</f>
-        <v>4051800</v>
-      </c>
-      <c r="G39" s="108"/>
-      <c r="H39" s="104"/>
-    </row>
-    <row r="40" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="82">
+      <c r="E51" s="158">
+        <f>SUM(B4:B41)</f>
+        <v>360825</v>
+      </c>
+      <c r="F51" s="84">
+        <f>E51*12</f>
+        <v>4329900</v>
+      </c>
+      <c r="G51" s="108"/>
+    </row>
+    <row r="52" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B52" s="82">
         <f>J7</f>
         <v>409000</v>
       </c>
-      <c r="C40" s="104" t="s">
+      <c r="C52" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="D40" s="172" t="s">
+      <c r="D52" s="172" t="s">
         <v>222</v>
       </c>
-      <c r="E40" s="84">
-        <f>SUM(B26:B31)</f>
+      <c r="E52" s="84">
+        <f>SUM(B43:B47)</f>
         <v>42000</v>
       </c>
-      <c r="F40" s="84">
-        <f>E40*12</f>
+      <c r="F52" s="84">
+        <f>E52*12</f>
         <v>504000</v>
       </c>
-      <c r="G40" s="108"/>
-      <c r="H40" s="104"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="83">
-        <f>B40-B39</f>
-        <v>29350</v>
-      </c>
-      <c r="C41" s="104" t="s">
+      <c r="G52" s="108"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="83">
+        <f>B52-B51</f>
+        <v>6175</v>
+      </c>
+      <c r="C53" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="15"/>
-      <c r="E41" s="168">
-        <f>SUM(E39:E40)</f>
-        <v>379650</v>
-      </c>
-      <c r="G41" s="108"/>
-      <c r="H41" s="104"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="168">
+        <f>SUM(E51:E52)</f>
+        <v>402825</v>
+      </c>
+      <c r="G53" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -8485,6 +8821,343 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34847FF8-7591-4C3B-8C24-D0E331C5B6A1}">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.85546875" style="117" customWidth="1"/>
+    <col min="2" max="2" width="17" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="119" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="84" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="57" customWidth="1"/>
+    <col min="8" max="8" width="18" style="113" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="227">
+        <v>44256</v>
+      </c>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+    </row>
+    <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="114"/>
+      <c r="B2" s="226" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="226"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="116"/>
+      <c r="B3" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="115" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="66" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="161">
+        <v>15000</v>
+      </c>
+      <c r="C4" s="121" t="s">
+        <v>287</v>
+      </c>
+      <c r="D4" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="56"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="161">
+        <v>27000</v>
+      </c>
+      <c r="C5" s="118" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="107" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="107" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="56"/>
+      <c r="G5" s="109"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="161">
+        <v>1500</v>
+      </c>
+      <c r="C6" s="118" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="107" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="107" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="161">
+        <v>1500</v>
+      </c>
+      <c r="C7" s="118" t="s">
+        <v>361</v>
+      </c>
+      <c r="D7" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="169" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="162">
+        <v>1500</v>
+      </c>
+      <c r="C8" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="119" t="s">
+        <v>363</v>
+      </c>
+      <c r="G9" s="108"/>
+      <c r="H9" s="104"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="119" t="s">
+        <v>355</v>
+      </c>
+      <c r="G10" s="108"/>
+      <c r="H10" s="104"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="108"/>
+      <c r="H11" s="104"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="108"/>
+      <c r="H12" s="104"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="108"/>
+      <c r="H13" s="104"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="108"/>
+      <c r="H14" s="104"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="108"/>
+      <c r="H15" s="104"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="108"/>
+      <c r="H16" s="104"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="108"/>
+      <c r="H17" s="104"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="108"/>
+      <c r="H18" s="104"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="145"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="104"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="145"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="104"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="165">
+        <v>10000</v>
+      </c>
+      <c r="C21" s="118" t="s">
+        <v>288</v>
+      </c>
+      <c r="D21" s="107" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="107" t="s">
+        <v>144</v>
+      </c>
+      <c r="G21" s="108"/>
+      <c r="H21" s="104"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="165">
+        <v>10000</v>
+      </c>
+      <c r="C22" s="118" t="s">
+        <v>289</v>
+      </c>
+      <c r="D22" s="169" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="169" t="s">
+        <v>149</v>
+      </c>
+      <c r="G22" s="108"/>
+      <c r="H22" s="104"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="165">
+        <v>3500</v>
+      </c>
+      <c r="C23" s="104" t="s">
+        <v>290</v>
+      </c>
+      <c r="D23" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="169" t="s">
+        <v>216</v>
+      </c>
+      <c r="G23" s="108"/>
+      <c r="H23" s="104"/>
+    </row>
+    <row r="24" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="166"/>
+      <c r="C24" s="104" t="s">
+        <v>298</v>
+      </c>
+      <c r="D24" s="143" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="143" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="166">
+        <v>22000</v>
+      </c>
+      <c r="C25" s="104" t="s">
+        <v>362</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="82">
+        <f>SUM(B4:B25)</f>
+        <v>92000</v>
+      </c>
+      <c r="C28" s="104" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="172" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" s="158">
+        <f>SUM(B4:B7)</f>
+        <v>45000</v>
+      </c>
+      <c r="F28" s="84">
+        <f>E28*12</f>
+        <v>540000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="82">
+        <v>85000</v>
+      </c>
+      <c r="C29" s="104" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="172" t="s">
+        <v>222</v>
+      </c>
+      <c r="E29" s="84">
+        <f>SUM(B21:B26)</f>
+        <v>45500</v>
+      </c>
+      <c r="F29" s="84">
+        <f>E29*12</f>
+        <v>546000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="83">
+        <f>B29-B28</f>
+        <v>-7000</v>
+      </c>
+      <c r="C30" s="104" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="168">
+        <f>SUM(E28:E29)</f>
+        <v>90500</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95534229-9251-45A5-AA67-E5DCE3AB28B0}">
   <dimension ref="A2:M17"/>
   <sheetViews>
@@ -8836,233 +9509,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BCBF0D-E6C2-4EAB-9EED-83649EF77F1B}">
-  <dimension ref="A1:I24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="35"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="33">
-        <v>43983</v>
-      </c>
-      <c r="B1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C1">
-        <v>16000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="33">
-        <v>43983</v>
-      </c>
-      <c r="B2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C2">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="34">
-        <v>43983</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="31">
-        <v>15000</v>
-      </c>
-      <c r="D3" s="31">
-        <f>SUM(C1:C3)</f>
-        <v>53000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
-        <v>44013</v>
-      </c>
-      <c r="B4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
-        <v>44013</v>
-      </c>
-      <c r="B5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="34">
-        <v>44013</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="C6" s="31">
-        <v>20000</v>
-      </c>
-      <c r="D6" s="31">
-        <f>SUM(C4:C6)</f>
-        <v>47000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="36">
-        <v>44044</v>
-      </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="36">
-        <v>44075</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="C8" s="32">
-        <v>17500</v>
-      </c>
-      <c r="D8" s="32">
-        <f t="shared" ref="D8:D13" si="0">SUM(C8)</f>
-        <v>17500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="36">
-        <v>44105</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="C9" s="32">
-        <v>15000</v>
-      </c>
-      <c r="D9" s="32">
-        <f t="shared" si="0"/>
-        <v>15000</v>
-      </c>
-      <c r="H9">
-        <v>9000</v>
-      </c>
-      <c r="I9">
-        <v>8500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="36">
-        <v>44136</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="C10" s="32">
-        <v>15000</v>
-      </c>
-      <c r="D10" s="32">
-        <f t="shared" si="0"/>
-        <v>15000</v>
-      </c>
-      <c r="H10">
-        <v>1148</v>
-      </c>
-      <c r="I10">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="37">
-        <v>44185</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>232</v>
-      </c>
-      <c r="C11" s="32">
-        <v>900</v>
-      </c>
-      <c r="D11" s="32">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="H11">
-        <f>SUM(H9:H10)</f>
-        <v>10148</v>
-      </c>
-      <c r="I11">
-        <f>SUM(I9:I10)</f>
-        <v>9648</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="36">
-        <v>44197</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="C12" s="32">
-        <v>15000</v>
-      </c>
-      <c r="D12" s="32">
-        <f t="shared" si="0"/>
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="36">
-        <v>44256</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="C13" s="32">
-        <v>17500</v>
-      </c>
-      <c r="D13" s="32">
-        <f t="shared" si="0"/>
-        <v>17500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C20" s="38">
-        <f>SUM(C1:C18)</f>
-        <v>180900</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="94" t="s">
-        <v>235</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39BCAFD-E759-4ED0-A2ED-96F522B36E8D}">
   <dimension ref="A1:I22"/>
@@ -9275,6 +9721,233 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BCBF0D-E6C2-4EAB-9EED-83649EF77F1B}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="35"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="33">
+        <v>43983</v>
+      </c>
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="33">
+        <v>43983</v>
+      </c>
+      <c r="B2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="34">
+        <v>43983</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="31">
+        <v>15000</v>
+      </c>
+      <c r="D3" s="31">
+        <f>SUM(C1:C3)</f>
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
+        <v>44013</v>
+      </c>
+      <c r="B4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
+        <v>44013</v>
+      </c>
+      <c r="B5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
+        <v>44013</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="31">
+        <v>20000</v>
+      </c>
+      <c r="D6" s="31">
+        <f>SUM(C4:C6)</f>
+        <v>47000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="36">
+        <v>44044</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>44075</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" s="32">
+        <v>17500</v>
+      </c>
+      <c r="D8" s="32">
+        <f t="shared" ref="D8:D13" si="0">SUM(C8)</f>
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="36">
+        <v>44105</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" s="32">
+        <v>15000</v>
+      </c>
+      <c r="D9" s="32">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+      <c r="H9">
+        <v>9000</v>
+      </c>
+      <c r="I9">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="36">
+        <v>44136</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C10" s="32">
+        <v>15000</v>
+      </c>
+      <c r="D10" s="32">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+      <c r="H10">
+        <v>1148</v>
+      </c>
+      <c r="I10">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="37">
+        <v>44185</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="32">
+        <v>900</v>
+      </c>
+      <c r="D11" s="32">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="H11">
+        <f>SUM(H9:H10)</f>
+        <v>10148</v>
+      </c>
+      <c r="I11">
+        <f>SUM(I9:I10)</f>
+        <v>9648</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="36">
+        <v>44197</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="C12" s="32">
+        <v>15000</v>
+      </c>
+      <c r="D12" s="32">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="36">
+        <v>44256</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13" s="32">
+        <v>17500</v>
+      </c>
+      <c r="D13" s="32">
+        <f t="shared" si="0"/>
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20" s="38">
+        <f>SUM(C1:C18)</f>
+        <v>180900</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="94" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CBCB0F-2985-4B71-8D89-BED119580876}">
   <dimension ref="A1:P21"/>
   <sheetViews>
@@ -9661,7 +10334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9AB30D-17DC-4D32-B251-C3E3B5456C1E}">
   <dimension ref="A1:F33"/>
   <sheetViews>
@@ -10056,7 +10729,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885679C4-12E3-4B74-819A-ABED6D5ACC2D}">
   <dimension ref="A2:H26"/>
   <sheetViews>
@@ -10162,7 +10835,7 @@
         <v>276</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D12" si="1">B5/12</f>
+        <f t="shared" ref="D5:D11" si="1">B5/12</f>
         <v>1250</v>
       </c>
       <c r="E5" s="22" t="s">
@@ -13572,21 +14245,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024D76020AE708242B68336FA618CBCDF" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0f8ef3af180fb4ddb5e95743212642f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df3f84f5-0dce-435a-abac-67420900ba59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2069e023351266972e9c1aca68960d8c" ns3:_="">
     <xsd:import namespace="df3f84f5-0dce-435a-abac-67420900ba59"/>
@@ -13756,24 +14414,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11DF5BFB-C4A2-42C5-9ACB-F42BB2AD57D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0955E539-E9CC-455F-B094-E363B2CCC487}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4845A164-C435-4094-8F0C-F88A8D76F182}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13789,4 +14445,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11DF5BFB-C4A2-42C5-9ACB-F42BB2AD57D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0955E539-E9CC-455F-B094-E363B2CCC487}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Budget_Home.xlsx Doc for April Month Expenses
</commit_message>
<xml_diff>
--- a/Budget_Home.xlsx
+++ b/Budget_Home.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Docs_Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130F5B3C-F647-4605-B38C-7F141C2BED9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BE2BA0-5C03-4CFE-A9C8-B7EB241C5FFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="820" firstSheet="13" activeTab="17" xr2:uid="{501F6562-0567-4B1B-9862-921E6A7B9365}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="820" firstSheet="13" activeTab="16" xr2:uid="{501F6562-0567-4B1B-9862-921E6A7B9365}"/>
   </bookViews>
   <sheets>
     <sheet name="LIC Details" sheetId="4" r:id="rId1"/>
@@ -437,7 +437,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="376">
   <si>
     <t>Value Date</t>
   </si>
@@ -1674,12 +1674,51 @@
   <si>
     <t>Mummy Medicines</t>
   </si>
+  <si>
+    <t>Roof</t>
+  </si>
+  <si>
+    <t>Servant Mumbai Home</t>
+  </si>
+  <si>
+    <t>Cash Withdrawal</t>
+  </si>
+  <si>
+    <t>Paid from LIC Loan
+Paid on 22 April '2021</t>
+  </si>
+  <si>
+    <t>Paid from LIC Loan
+Paid on 24 April '2021</t>
+  </si>
+  <si>
+    <t>Cab to Pune (Rupal &amp; Prisha)</t>
+  </si>
+  <si>
+    <t>Mummy Bosy Cleaning….Bai</t>
+  </si>
+  <si>
+    <t>Mobile Purchase</t>
+  </si>
+  <si>
+    <t>Paid from LIC Loan
+Paid on 23 April '2021</t>
+  </si>
+  <si>
+    <t>Cab to Pune ( Mummy &amp; Papa )</t>
+  </si>
+  <si>
+    <t>Gillete Blade &amp; Razor ( D'Mart )</t>
+  </si>
+  <si>
+    <t>Dettol Spray + Dettol Sanitizer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1845,12 +1884,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2561,6 +2594,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2572,24 +2623,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3620,99 +3653,104 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="211">
+      <c r="A9" s="217">
         <v>3</v>
       </c>
-      <c r="B9" s="213" t="s">
+      <c r="B9" s="219" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="213" t="s">
+      <c r="C9" s="219" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="215"/>
+      <c r="D9" s="213"/>
       <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="217">
+      <c r="F9" s="215">
         <v>5800</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="212"/>
-      <c r="B10" s="214"/>
-      <c r="C10" s="214"/>
-      <c r="D10" s="216"/>
+      <c r="A10" s="218"/>
+      <c r="B10" s="220"/>
+      <c r="C10" s="220"/>
+      <c r="D10" s="214"/>
       <c r="E10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="218"/>
+      <c r="F10" s="216"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="211">
+      <c r="A11" s="217">
         <v>15</v>
       </c>
-      <c r="B11" s="213" t="s">
+      <c r="B11" s="219" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="213" t="s">
+      <c r="C11" s="219" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="215"/>
+      <c r="D11" s="213"/>
       <c r="E11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="217">
+      <c r="F11" s="215">
         <v>5800</v>
       </c>
-      <c r="G11" s="219"/>
-      <c r="H11" s="217"/>
+      <c r="G11" s="211"/>
+      <c r="H11" s="215"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="212"/>
-      <c r="B12" s="214"/>
-      <c r="C12" s="214"/>
-      <c r="D12" s="216"/>
+      <c r="A12" s="218"/>
+      <c r="B12" s="220"/>
+      <c r="C12" s="220"/>
+      <c r="D12" s="214"/>
       <c r="E12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="218"/>
-      <c r="G12" s="220"/>
-      <c r="H12" s="218"/>
+      <c r="F12" s="216"/>
+      <c r="G12" s="212"/>
+      <c r="H12" s="216"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="211">
+      <c r="A13" s="217">
         <v>16</v>
       </c>
-      <c r="B13" s="213" t="s">
+      <c r="B13" s="219" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="213" t="s">
+      <c r="C13" s="219" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="215"/>
+      <c r="D13" s="213"/>
       <c r="E13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="217">
+      <c r="F13" s="215">
         <v>5800</v>
       </c>
-      <c r="G13" s="219"/>
-      <c r="H13" s="217"/>
+      <c r="G13" s="211"/>
+      <c r="H13" s="215"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="212"/>
-      <c r="B14" s="214"/>
-      <c r="C14" s="214"/>
-      <c r="D14" s="216"/>
+      <c r="A14" s="218"/>
+      <c r="B14" s="220"/>
+      <c r="C14" s="220"/>
+      <c r="D14" s="214"/>
       <c r="E14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="218"/>
-      <c r="G14" s="220"/>
-      <c r="H14" s="218"/>
+      <c r="F14" s="216"/>
+      <c r="G14" s="212"/>
+      <c r="H14" s="216"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="H11:H12"/>
@@ -3727,11 +3765,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7944,8 +7977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF25BCD7-403F-4682-8C4D-9874D3ECF04E}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8602,36 +8635,167 @@
       </c>
       <c r="H30" s="104"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="82"/>
-      <c r="G31" s="110"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="82"/>
-      <c r="G32" s="110"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="82"/>
-      <c r="G33" s="110"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="82"/>
-      <c r="G34" s="110"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="82"/>
-      <c r="G35" s="110"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="82"/>
-      <c r="G36" s="110"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G37" s="110"/>
+    <row r="31" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="82">
+        <v>8000</v>
+      </c>
+      <c r="C31" s="119" t="s">
+        <v>364</v>
+      </c>
+      <c r="D31" s="143" t="s">
+        <v>216</v>
+      </c>
+      <c r="E31" s="143" t="s">
+        <v>181</v>
+      </c>
+      <c r="F31" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="110" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="82">
+        <v>3800</v>
+      </c>
+      <c r="C32" s="119" t="s">
+        <v>365</v>
+      </c>
+      <c r="D32" s="143" t="s">
+        <v>216</v>
+      </c>
+      <c r="E32" s="143" t="s">
+        <v>366</v>
+      </c>
+      <c r="F32" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="110" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="82">
+        <v>2050</v>
+      </c>
+      <c r="C33" s="119" t="s">
+        <v>369</v>
+      </c>
+      <c r="D33" s="143" t="s">
+        <v>216</v>
+      </c>
+      <c r="E33" s="143" t="s">
+        <v>366</v>
+      </c>
+      <c r="F33" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="110" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="82">
+        <v>1000</v>
+      </c>
+      <c r="C34" s="119" t="s">
+        <v>370</v>
+      </c>
+      <c r="D34" s="143" t="s">
+        <v>216</v>
+      </c>
+      <c r="E34" s="143" t="s">
+        <v>366</v>
+      </c>
+      <c r="F34" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="110" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="82">
+        <v>16500</v>
+      </c>
+      <c r="C35" s="119" t="s">
+        <v>371</v>
+      </c>
+      <c r="D35" s="143" t="s">
+        <v>216</v>
+      </c>
+      <c r="E35" s="143" t="s">
+        <v>366</v>
+      </c>
+      <c r="F35" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="110" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="82">
+        <v>3500</v>
+      </c>
+      <c r="C36" s="119" t="s">
+        <v>373</v>
+      </c>
+      <c r="D36" s="143" t="s">
+        <v>216</v>
+      </c>
+      <c r="E36" s="143" t="s">
+        <v>366</v>
+      </c>
+      <c r="F36" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="110" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="82">
+        <v>2000</v>
+      </c>
+      <c r="C37" s="119" t="s">
+        <v>374</v>
+      </c>
+      <c r="D37" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="110" t="s">
+        <v>337</v>
+      </c>
       <c r="H37" s="104"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G38" s="110"/>
+    <row r="38" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="82">
+        <f>225+235</f>
+        <v>460</v>
+      </c>
+      <c r="C38" s="119" t="s">
+        <v>375</v>
+      </c>
+      <c r="D38" s="143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="110" t="s">
+        <v>337</v>
+      </c>
       <c r="H38" s="104"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -8754,7 +8918,7 @@
     <row r="51" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="82">
         <f>SUM(B4:B49)</f>
-        <v>402825</v>
+        <v>440135</v>
       </c>
       <c r="C51" s="104" t="s">
         <v>31</v>
@@ -8764,11 +8928,11 @@
       </c>
       <c r="E51" s="158">
         <f>SUM(B4:B41)</f>
-        <v>360825</v>
+        <v>398135</v>
       </c>
       <c r="F51" s="84">
         <f>E51*12</f>
-        <v>4329900</v>
+        <v>4777620</v>
       </c>
       <c r="G51" s="108"/>
     </row>
@@ -8796,7 +8960,7 @@
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="83">
         <f>B52-B51</f>
-        <v>6175</v>
+        <v>-31135</v>
       </c>
       <c r="C53" s="104" t="s">
         <v>108</v>
@@ -8804,7 +8968,7 @@
       <c r="D53" s="15"/>
       <c r="E53" s="168">
         <f>SUM(E51:E52)</f>
-        <v>402825</v>
+        <v>440135</v>
       </c>
       <c r="G53" s="108"/>
     </row>
@@ -8824,7 +8988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34847FF8-7591-4C3B-8C24-D0E331C5B6A1}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -14245,6 +14409,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024D76020AE708242B68336FA618CBCDF" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0f8ef3af180fb4ddb5e95743212642f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df3f84f5-0dce-435a-abac-67420900ba59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2069e023351266972e9c1aca68960d8c" ns3:_="">
     <xsd:import namespace="df3f84f5-0dce-435a-abac-67420900ba59"/>
@@ -14414,22 +14593,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0955E539-E9CC-455F-B094-E363B2CCC487}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11DF5BFB-C4A2-42C5-9ACB-F42BB2AD57D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4845A164-C435-4094-8F0C-F88A8D76F182}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14445,21 +14626,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11DF5BFB-C4A2-42C5-9ACB-F42BB2AD57D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0955E539-E9CC-455F-B094-E363B2CCC487}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Expenses in Budget Home Doc
</commit_message>
<xml_diff>
--- a/Budget_Home.xlsx
+++ b/Budget_Home.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Docs_Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BE2BA0-5C03-4CFE-A9C8-B7EB241C5FFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BB0ADD-FA05-4030-93C0-7FF9DAE03114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="820" firstSheet="13" activeTab="16" xr2:uid="{501F6562-0567-4B1B-9862-921E6A7B9365}"/>
   </bookViews>
@@ -437,7 +437,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="380">
   <si>
     <t>Value Date</t>
   </si>
@@ -1712,6 +1712,18 @@
   </si>
   <si>
     <t>Dettol Spray + Dettol Sanitizer</t>
+  </si>
+  <si>
+    <t>Snacks for mom dad</t>
+  </si>
+  <si>
+    <t>Papa Report at evening</t>
+  </si>
+  <si>
+    <t>Medicines</t>
+  </si>
+  <si>
+    <t>Petrol Mahek Bike</t>
   </si>
 </sst>
 </file>
@@ -2594,35 +2606,35 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3028,13 +3040,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1095375</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3653,104 +3665,99 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="217">
+      <c r="A9" s="211">
         <v>3</v>
       </c>
-      <c r="B9" s="219" t="s">
+      <c r="B9" s="213" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="219" t="s">
+      <c r="C9" s="213" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="213"/>
+      <c r="D9" s="215"/>
       <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="215">
+      <c r="F9" s="217">
         <v>5800</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="218"/>
-      <c r="B10" s="220"/>
-      <c r="C10" s="220"/>
-      <c r="D10" s="214"/>
+      <c r="A10" s="212"/>
+      <c r="B10" s="214"/>
+      <c r="C10" s="214"/>
+      <c r="D10" s="216"/>
       <c r="E10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="216"/>
+      <c r="F10" s="218"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="217">
+      <c r="A11" s="211">
         <v>15</v>
       </c>
-      <c r="B11" s="219" t="s">
+      <c r="B11" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="219" t="s">
+      <c r="C11" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="213"/>
+      <c r="D11" s="215"/>
       <c r="E11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="215">
+      <c r="F11" s="217">
         <v>5800</v>
       </c>
-      <c r="G11" s="211"/>
-      <c r="H11" s="215"/>
+      <c r="G11" s="219"/>
+      <c r="H11" s="217"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="218"/>
-      <c r="B12" s="220"/>
-      <c r="C12" s="220"/>
-      <c r="D12" s="214"/>
+      <c r="A12" s="212"/>
+      <c r="B12" s="214"/>
+      <c r="C12" s="214"/>
+      <c r="D12" s="216"/>
       <c r="E12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="216"/>
-      <c r="G12" s="212"/>
-      <c r="H12" s="216"/>
+      <c r="F12" s="218"/>
+      <c r="G12" s="220"/>
+      <c r="H12" s="218"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="217">
+      <c r="A13" s="211">
         <v>16</v>
       </c>
-      <c r="B13" s="219" t="s">
+      <c r="B13" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="219" t="s">
+      <c r="C13" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="213"/>
+      <c r="D13" s="215"/>
       <c r="E13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="215">
+      <c r="F13" s="217">
         <v>5800</v>
       </c>
-      <c r="G13" s="211"/>
-      <c r="H13" s="215"/>
+      <c r="G13" s="219"/>
+      <c r="H13" s="217"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="218"/>
-      <c r="B14" s="220"/>
-      <c r="C14" s="220"/>
-      <c r="D14" s="214"/>
+      <c r="A14" s="212"/>
+      <c r="B14" s="214"/>
+      <c r="C14" s="214"/>
+      <c r="D14" s="216"/>
       <c r="E14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="216"/>
-      <c r="G14" s="212"/>
-      <c r="H14" s="216"/>
+      <c r="F14" s="218"/>
+      <c r="G14" s="220"/>
+      <c r="H14" s="218"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="H11:H12"/>
@@ -3765,6 +3772,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7975,10 +7987,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF25BCD7-403F-4682-8C4D-9874D3ECF04E}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8799,19 +8811,87 @@
       <c r="H38" s="104"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G39" s="110"/>
+      <c r="B39" s="82">
+        <v>500</v>
+      </c>
+      <c r="C39" s="119" t="s">
+        <v>376</v>
+      </c>
+      <c r="D39" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="143" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="110" t="s">
+        <v>337</v>
+      </c>
       <c r="H39" s="104"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G40" s="110"/>
+      <c r="B40" s="82">
+        <v>1250</v>
+      </c>
+      <c r="C40" s="119" t="s">
+        <v>377</v>
+      </c>
+      <c r="D40" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="110" t="s">
+        <v>337</v>
+      </c>
       <c r="H40" s="104"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G41" s="110"/>
+      <c r="B41" s="82">
+        <v>2000</v>
+      </c>
+      <c r="C41" s="119" t="s">
+        <v>378</v>
+      </c>
+      <c r="D41" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="143" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="110" t="s">
+        <v>232</v>
+      </c>
       <c r="H41" s="104"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G42" s="110"/>
+      <c r="B42" s="82">
+        <v>150</v>
+      </c>
+      <c r="C42" s="119" t="s">
+        <v>379</v>
+      </c>
+      <c r="D42" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="143" t="s">
+        <v>36</v>
+      </c>
+      <c r="F42" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="110" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="165">
@@ -8826,7 +8906,12 @@
       <c r="E43" s="107" t="s">
         <v>144</v>
       </c>
-      <c r="G43" s="108"/>
+      <c r="F43" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="110" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="165">
@@ -8841,7 +8926,12 @@
       <c r="E44" s="169" t="s">
         <v>149</v>
       </c>
-      <c r="G44" s="108"/>
+      <c r="F44" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="110" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="165">
@@ -8859,46 +8949,40 @@
       <c r="F45" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="G45" s="108"/>
-    </row>
-    <row r="46" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G45" s="108" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="166">
-        <v>15000</v>
+        <v>3500</v>
       </c>
       <c r="C46" s="104" t="s">
-        <v>298</v>
+        <v>191</v>
       </c>
       <c r="D46" s="143" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E46" s="143" t="s">
-        <v>291</v>
-      </c>
-      <c r="G46" s="108"/>
+        <v>191</v>
+      </c>
+      <c r="F46" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" s="108" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="166">
-        <v>3500</v>
-      </c>
-      <c r="C47" s="104" t="s">
-        <v>191</v>
-      </c>
-      <c r="D47" s="143" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="143" t="s">
-        <v>191</v>
-      </c>
-      <c r="F47" s="84" t="s">
-        <v>17</v>
-      </c>
-      <c r="G47" s="108" t="s">
-        <v>324</v>
-      </c>
+      <c r="B47" s="83"/>
+      <c r="C47" s="104"/>
+      <c r="G47" s="108"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="83"/>
-      <c r="C48" s="104"/>
+      <c r="B48" s="145"/>
+      <c r="C48" s="118"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
       <c r="G48" s="108"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
@@ -8908,69 +8992,62 @@
       <c r="E49" s="15"/>
       <c r="G49" s="108"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="145"/>
-      <c r="C50" s="118"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
+    <row r="50" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="82">
+        <f>SUM(B4:B48)</f>
+        <v>429035</v>
+      </c>
+      <c r="C50" s="104" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="172" t="s">
+        <v>221</v>
+      </c>
+      <c r="E50" s="158">
+        <f>SUM(B4:B41)</f>
+        <v>401885</v>
+      </c>
+      <c r="F50" s="84">
+        <f>E50*12</f>
+        <v>4822620</v>
+      </c>
       <c r="G50" s="108"/>
     </row>
     <row r="51" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="82">
-        <f>SUM(B4:B49)</f>
-        <v>440135</v>
+        <f>J7</f>
+        <v>409000</v>
       </c>
       <c r="C51" s="104" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D51" s="172" t="s">
-        <v>221</v>
-      </c>
-      <c r="E51" s="158">
-        <f>SUM(B4:B41)</f>
-        <v>398135</v>
+        <v>222</v>
+      </c>
+      <c r="E51" s="84">
+        <f>SUM(B43:B46)</f>
+        <v>27000</v>
       </c>
       <c r="F51" s="84">
         <f>E51*12</f>
-        <v>4777620</v>
+        <v>324000</v>
       </c>
       <c r="G51" s="108"/>
     </row>
-    <row r="52" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="82">
-        <f>J7</f>
-        <v>409000</v>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="83">
+        <f>B51-B50</f>
+        <v>-20035</v>
       </c>
       <c r="C52" s="104" t="s">
-        <v>66</v>
-      </c>
-      <c r="D52" s="172" t="s">
-        <v>222</v>
-      </c>
-      <c r="E52" s="84">
-        <f>SUM(B43:B47)</f>
-        <v>42000</v>
-      </c>
-      <c r="F52" s="84">
-        <f>E52*12</f>
-        <v>504000</v>
+        <v>108</v>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="168">
+        <f>SUM(E50:E51)</f>
+        <v>428885</v>
       </c>
       <c r="G52" s="108"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="83">
-        <f>B52-B51</f>
-        <v>-31135</v>
-      </c>
-      <c r="C53" s="104" t="s">
-        <v>108</v>
-      </c>
-      <c r="D53" s="15"/>
-      <c r="E53" s="168">
-        <f>SUM(E51:E52)</f>
-        <v>440135</v>
-      </c>
-      <c r="G53" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -14409,21 +14486,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024D76020AE708242B68336FA618CBCDF" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0f8ef3af180fb4ddb5e95743212642f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df3f84f5-0dce-435a-abac-67420900ba59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2069e023351266972e9c1aca68960d8c" ns3:_="">
     <xsd:import namespace="df3f84f5-0dce-435a-abac-67420900ba59"/>
@@ -14593,24 +14655,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0955E539-E9CC-455F-B094-E363B2CCC487}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11DF5BFB-C4A2-42C5-9ACB-F42BB2AD57D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4845A164-C435-4094-8F0C-F88A8D76F182}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14626,4 +14686,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11DF5BFB-C4A2-42C5-9ACB-F42BB2AD57D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0955E539-E9CC-455F-B094-E363B2CCC487}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated budget excel doc
</commit_message>
<xml_diff>
--- a/Budget_Home.xlsx
+++ b/Budget_Home.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Jimish\personal\Docs_Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A23F3F1-1D56-4DBB-8250-8171A207E36C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB675C19-02F6-44B0-B2FB-468C54D66345}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="820" firstSheet="13" activeTab="25" xr2:uid="{501F6562-0567-4B1B-9862-921E6A7B9365}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="820" firstSheet="13" activeTab="23" xr2:uid="{501F6562-0567-4B1B-9862-921E6A7B9365}"/>
   </bookViews>
   <sheets>
     <sheet name="LIC Details" sheetId="4" r:id="rId1"/>
@@ -1847,9 +1847,6 @@
     <t>Prisha Pocket Money</t>
   </si>
   <si>
-    <t>Prisha Fees</t>
-  </si>
-  <si>
     <t>Tiffin</t>
   </si>
   <si>
@@ -1902,6 +1899,9 @@
   </si>
   <si>
     <t>5th installment</t>
+  </si>
+  <si>
+    <t>Prisha School Fees - Last installment</t>
   </si>
 </sst>
 </file>
@@ -2831,11 +2831,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2849,17 +2858,11 @@
     <xf numFmtId="4" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2896,9 +2899,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4349,104 +4349,99 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="235">
+      <c r="A9" s="230">
         <v>3</v>
       </c>
-      <c r="B9" s="237" t="s">
+      <c r="B9" s="232" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="237" t="s">
+      <c r="C9" s="232" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="231"/>
+      <c r="D9" s="234"/>
       <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="233">
+      <c r="F9" s="236">
         <v>5800</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="236"/>
-      <c r="B10" s="238"/>
-      <c r="C10" s="238"/>
-      <c r="D10" s="232"/>
+      <c r="A10" s="231"/>
+      <c r="B10" s="233"/>
+      <c r="C10" s="233"/>
+      <c r="D10" s="235"/>
       <c r="E10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="234"/>
+      <c r="F10" s="237"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="235">
+      <c r="A11" s="230">
         <v>15</v>
       </c>
-      <c r="B11" s="237" t="s">
+      <c r="B11" s="232" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="237" t="s">
+      <c r="C11" s="232" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="231"/>
+      <c r="D11" s="234"/>
       <c r="E11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="233">
+      <c r="F11" s="236">
         <v>5800</v>
       </c>
-      <c r="G11" s="229"/>
-      <c r="H11" s="233"/>
+      <c r="G11" s="238"/>
+      <c r="H11" s="236"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="236"/>
-      <c r="B12" s="238"/>
-      <c r="C12" s="238"/>
-      <c r="D12" s="232"/>
+      <c r="A12" s="231"/>
+      <c r="B12" s="233"/>
+      <c r="C12" s="233"/>
+      <c r="D12" s="235"/>
       <c r="E12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="234"/>
-      <c r="G12" s="230"/>
-      <c r="H12" s="234"/>
+      <c r="F12" s="237"/>
+      <c r="G12" s="239"/>
+      <c r="H12" s="237"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="235">
+      <c r="A13" s="230">
         <v>16</v>
       </c>
-      <c r="B13" s="237" t="s">
+      <c r="B13" s="232" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="237" t="s">
+      <c r="C13" s="232" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="231"/>
+      <c r="D13" s="234"/>
       <c r="E13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="233">
+      <c r="F13" s="236">
         <v>5800</v>
       </c>
-      <c r="G13" s="229"/>
-      <c r="H13" s="233"/>
+      <c r="G13" s="238"/>
+      <c r="H13" s="236"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="236"/>
-      <c r="B14" s="238"/>
-      <c r="C14" s="238"/>
-      <c r="D14" s="232"/>
+      <c r="A14" s="231"/>
+      <c r="B14" s="233"/>
+      <c r="C14" s="233"/>
+      <c r="D14" s="235"/>
       <c r="E14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="234"/>
-      <c r="G14" s="230"/>
-      <c r="H14" s="234"/>
+      <c r="F14" s="237"/>
+      <c r="G14" s="239"/>
+      <c r="H14" s="237"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="H11:H12"/>
@@ -4461,6 +4456,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4494,40 +4494,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44075</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="246"/>
+      <c r="J1" s="246"/>
+      <c r="K1" s="246"/>
+      <c r="L1" s="246"/>
+      <c r="M1" s="246"/>
     </row>
     <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="243" t="s">
+      <c r="A2" s="244" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
-      <c r="F2" s="243"/>
+      <c r="B2" s="244"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="244"/>
+      <c r="E2" s="244"/>
+      <c r="F2" s="244"/>
       <c r="G2" s="114"/>
-      <c r="H2" s="244" t="s">
+      <c r="H2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
-      <c r="M2" s="244"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="245"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -5230,38 +5230,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44105</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="246"/>
+      <c r="J1" s="246"/>
+      <c r="K1" s="246"/>
+      <c r="L1" s="246"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="243" t="s">
+      <c r="A2" s="244" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
+      <c r="B2" s="244"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="244"/>
+      <c r="E2" s="244"/>
       <c r="F2" s="114"/>
-      <c r="G2" s="244" t="s">
+      <c r="G2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -5922,38 +5922,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44136</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="246"/>
+      <c r="J1" s="246"/>
+      <c r="K1" s="246"/>
+      <c r="L1" s="246"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="243" t="s">
+      <c r="A2" s="244" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
+      <c r="B2" s="244"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="244"/>
+      <c r="E2" s="244"/>
       <c r="F2" s="114"/>
-      <c r="G2" s="244" t="s">
+      <c r="G2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -6623,38 +6623,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44166</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="246"/>
+      <c r="J1" s="246"/>
+      <c r="K1" s="246"/>
+      <c r="L1" s="246"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="243" t="s">
+      <c r="A2" s="244" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
+      <c r="B2" s="244"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="244"/>
+      <c r="E2" s="244"/>
       <c r="F2" s="114"/>
-      <c r="G2" s="244" t="s">
+      <c r="G2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -7324,38 +7324,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="246" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="246"/>
+      <c r="J1" s="246"/>
+      <c r="K1" s="246"/>
+      <c r="L1" s="246"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="243" t="s">
+      <c r="A2" s="244" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
+      <c r="B2" s="244"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="244"/>
+      <c r="E2" s="244"/>
       <c r="F2" s="114"/>
-      <c r="G2" s="244" t="s">
+      <c r="G2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -7986,26 +7986,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44228</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="116"/>
@@ -8343,26 +8343,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44256</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="116"/>
@@ -8693,26 +8693,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44287</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
     </row>
     <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="116"/>
@@ -8734,10 +8734,10 @@
       <c r="G3" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="I3" s="246" t="s">
+      <c r="I3" s="247" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="246"/>
+      <c r="J3" s="247"/>
       <c r="K3" s="195" t="s">
         <v>331</v>
       </c>
@@ -9846,26 +9846,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44317</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="116"/>
@@ -10205,26 +10205,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44348</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="116"/>
@@ -10584,12 +10584,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="239" t="s">
+      <c r="B1" s="240" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
       <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
@@ -10800,26 +10800,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44378</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="116"/>
@@ -11134,27 +11134,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44470</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
       <c r="H1" s="113"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
       <c r="H2" s="113"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -11409,7 +11409,7 @@
         <v>421</v>
       </c>
       <c r="G17" s="112" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H17" s="104"/>
     </row>
@@ -11546,27 +11546,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44501</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
       <c r="H1" s="113"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
       <c r="H2" s="113"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -11783,7 +11783,7 @@
         <v>421</v>
       </c>
       <c r="G17" s="112" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H17" s="104"/>
     </row>
@@ -11920,27 +11920,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44531</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
       <c r="H1" s="113"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
       <c r="H2" s="113"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -11982,7 +11982,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="221" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H4" s="113"/>
     </row>
@@ -12003,7 +12003,7 @@
         <v>17</v>
       </c>
       <c r="G5" s="221" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H5" s="113"/>
     </row>
@@ -12024,7 +12024,7 @@
         <v>17</v>
       </c>
       <c r="G6" s="221" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H6" s="113"/>
     </row>
@@ -12033,7 +12033,7 @@
         <v>3650</v>
       </c>
       <c r="C7" s="104" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D7" s="143" t="s">
         <v>35</v>
@@ -12062,7 +12062,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="221" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H8" s="113"/>
     </row>
@@ -12083,7 +12083,7 @@
         <v>17</v>
       </c>
       <c r="G9" s="228" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H9" s="104"/>
     </row>
@@ -12098,13 +12098,13 @@
         <v>35</v>
       </c>
       <c r="E10" s="169" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F10" s="84" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="228" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H10" s="104"/>
     </row>
@@ -12113,7 +12113,7 @@
         <v>350</v>
       </c>
       <c r="C11" s="104" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D11" s="227" t="s">
         <v>35</v>
@@ -12125,7 +12125,7 @@
         <v>17</v>
       </c>
       <c r="G11" s="228" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H11" s="104"/>
     </row>
@@ -12146,7 +12146,7 @@
         <v>17</v>
       </c>
       <c r="G12" s="221" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H12" s="104"/>
     </row>
@@ -12167,7 +12167,7 @@
         <v>17</v>
       </c>
       <c r="G13" s="221" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H13" s="104"/>
     </row>
@@ -12188,7 +12188,7 @@
         <v>17</v>
       </c>
       <c r="G14" s="228" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H14" s="104"/>
     </row>
@@ -12223,10 +12223,10 @@
       <c r="H19" s="113"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E20" s="247" t="s">
+      <c r="E20" s="248" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="247"/>
+      <c r="F20" s="248"/>
       <c r="G20" s="221"/>
       <c r="H20" s="113"/>
     </row>
@@ -12307,8 +12307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B98ADB7-38FA-48C9-8F78-9514EF2C75AE}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12323,27 +12323,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44562</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
       <c r="H1" s="113"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
       <c r="H2" s="113"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -12385,7 +12385,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="221" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H4" s="113"/>
     </row>
@@ -12425,7 +12425,7 @@
         <v>17</v>
       </c>
       <c r="G6" s="221" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H6" s="113"/>
     </row>
@@ -12434,7 +12434,7 @@
         <v>14875</v>
       </c>
       <c r="C7" s="104" t="s">
-        <v>424</v>
+        <v>442</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>35</v>
@@ -12445,8 +12445,8 @@
       <c r="F7" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="251" t="s">
-        <v>435</v>
+      <c r="G7" s="229" t="s">
+        <v>434</v>
       </c>
       <c r="H7" s="113"/>
     </row>
@@ -12467,7 +12467,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="112" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H8" s="104"/>
     </row>
@@ -12495,7 +12495,7 @@
         <v>1800</v>
       </c>
       <c r="C10" s="104" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D10" s="57" t="s">
         <v>35</v>
@@ -12507,7 +12507,7 @@
         <v>17</v>
       </c>
       <c r="G10" s="224" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H10" s="104"/>
     </row>
@@ -12516,7 +12516,7 @@
         <v>3000</v>
       </c>
       <c r="C11" s="119" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D11" s="57" t="s">
         <v>35</v>
@@ -12528,7 +12528,7 @@
         <v>17</v>
       </c>
       <c r="G11" s="224" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H11" s="104"/>
     </row>
@@ -12577,7 +12577,7 @@
         <v>17</v>
       </c>
       <c r="G14" s="112" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H14" s="104"/>
     </row>
@@ -12598,7 +12598,7 @@
         <v>17</v>
       </c>
       <c r="G15" s="112" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H15" s="104"/>
     </row>
@@ -12633,10 +12633,10 @@
       <c r="H20" s="113"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="247" t="s">
+      <c r="D21" s="248" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="247"/>
+      <c r="E21" s="248"/>
       <c r="F21" s="84"/>
       <c r="G21" s="221"/>
       <c r="H21" s="113"/>
@@ -12734,27 +12734,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44593</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
       <c r="H1" s="113"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
       <c r="H2" s="113"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -12794,7 +12794,7 @@
       </c>
       <c r="F4" s="56"/>
       <c r="G4" s="221" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H4" s="113"/>
     </row>
@@ -12830,7 +12830,7 @@
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="221" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H6" s="113"/>
     </row>
@@ -12840,7 +12840,7 @@
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="56"/>
-      <c r="G7" s="251"/>
+      <c r="G7" s="229"/>
       <c r="H7" s="113"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -12858,7 +12858,7 @@
       </c>
       <c r="F8" s="56"/>
       <c r="G8" s="112" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H8" s="104"/>
     </row>
@@ -12882,7 +12882,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="82"/>
       <c r="C10" s="104" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D10" s="57" t="s">
         <v>35</v>
@@ -12892,14 +12892,14 @@
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="224" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H10" s="104"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="82"/>
       <c r="C11" s="119" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D11" s="57" t="s">
         <v>35</v>
@@ -12909,7 +12909,7 @@
       </c>
       <c r="F11" s="56"/>
       <c r="G11" s="224" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H11" s="104"/>
     </row>
@@ -12954,7 +12954,7 @@
       </c>
       <c r="F14" s="84"/>
       <c r="G14" s="112" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H14" s="104"/>
     </row>
@@ -12973,7 +12973,7 @@
       </c>
       <c r="F15" s="84"/>
       <c r="G15" s="112" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H15" s="104"/>
     </row>
@@ -13008,10 +13008,10 @@
       <c r="H20" s="113"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="247" t="s">
+      <c r="D21" s="248" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="247"/>
+      <c r="E21" s="248"/>
       <c r="F21" s="84"/>
       <c r="G21" s="221"/>
       <c r="H21" s="113"/>
@@ -13093,8 +13093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDE23A1-3A6E-47D7-B0A6-FAEC05C07672}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13109,27 +13109,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="245">
+      <c r="A1" s="246">
         <v>44621</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
       <c r="H1" s="113"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="114"/>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="245"/>
+      <c r="F2" s="245"/>
+      <c r="G2" s="245"/>
       <c r="H2" s="113"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -13169,7 +13169,7 @@
       </c>
       <c r="F4" s="56"/>
       <c r="G4" s="221" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H4" s="113"/>
     </row>
@@ -13205,7 +13205,7 @@
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="221" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H6" s="113"/>
     </row>
@@ -13221,7 +13221,7 @@
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="56"/>
-      <c r="G7" s="251"/>
+      <c r="G7" s="229"/>
       <c r="H7" s="113"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -13239,7 +13239,7 @@
       </c>
       <c r="F8" s="56"/>
       <c r="G8" s="112" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H8" s="104"/>
     </row>
@@ -13312,7 +13312,7 @@
       </c>
       <c r="F14" s="84"/>
       <c r="G14" s="112" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H14" s="104"/>
     </row>
@@ -13331,7 +13331,7 @@
       </c>
       <c r="F15" s="84"/>
       <c r="G15" s="112" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H15" s="104"/>
     </row>
@@ -13366,10 +13366,10 @@
       <c r="H20" s="113"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="247" t="s">
+      <c r="D21" s="248" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="247"/>
+      <c r="E21" s="248"/>
       <c r="F21" s="84"/>
       <c r="G21" s="221"/>
       <c r="H21" s="113"/>
@@ -13463,11 +13463,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="239" t="s">
+      <c r="B1" s="240" t="s">
         <v>387</v>
       </c>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="151" t="s">
@@ -13712,7 +13712,7 @@
       <c r="E2" s="192" t="s">
         <v>303</v>
       </c>
-      <c r="F2" s="248"/>
+      <c r="F2" s="249"/>
       <c r="G2" s="151" t="s">
         <v>301</v>
       </c>
@@ -13739,7 +13739,7 @@
       <c r="E3" s="1">
         <v>2000</v>
       </c>
-      <c r="F3" s="248"/>
+      <c r="F3" s="249"/>
       <c r="G3" s="209" t="s">
         <v>304</v>
       </c>
@@ -14271,12 +14271,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="239" t="s">
+      <c r="B1" s="240" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
       <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
@@ -14969,13 +14969,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="249" t="s">
+      <c r="A1" s="250" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="249"/>
-      <c r="C1" s="249"/>
-      <c r="D1" s="249"/>
-      <c r="E1" s="250"/>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="251"/>
     </row>
     <row r="2" spans="1:6" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="137">
@@ -15694,12 +15694,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="239" t="s">
+      <c r="B1" s="240" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
       <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
@@ -16119,12 +16119,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="239" t="s">
+      <c r="B1" s="240" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
       <c r="F1" s="3"/>
       <c r="G1" s="2"/>
       <c r="I1" s="5">
@@ -16443,14 +16443,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="240">
+      <c r="A1" s="241">
         <v>43952</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
       <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -16778,14 +16778,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="240">
+      <c r="A1" s="241">
         <v>43983</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
       <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -17261,40 +17261,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="240">
+      <c r="A1" s="241">
         <v>44013</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="241"/>
+      <c r="I1" s="241"/>
+      <c r="J1" s="241"/>
+      <c r="K1" s="241"/>
+      <c r="L1" s="241"/>
+      <c r="M1" s="241"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="241" t="s">
+      <c r="A2" s="242" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="241"/>
-      <c r="C2" s="241"/>
-      <c r="D2" s="241"/>
-      <c r="E2" s="241"/>
-      <c r="F2" s="241"/>
+      <c r="B2" s="242"/>
+      <c r="C2" s="242"/>
+      <c r="D2" s="242"/>
+      <c r="E2" s="242"/>
+      <c r="F2" s="242"/>
       <c r="G2" s="88"/>
-      <c r="H2" s="242" t="s">
+      <c r="H2" s="243" t="s">
         <v>133</v>
       </c>
-      <c r="I2" s="242"/>
-      <c r="J2" s="242"/>
-      <c r="K2" s="242"/>
-      <c r="L2" s="242"/>
-      <c r="M2" s="242"/>
+      <c r="I2" s="243"/>
+      <c r="J2" s="243"/>
+      <c r="K2" s="243"/>
+      <c r="L2" s="243"/>
+      <c r="M2" s="243"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -17860,38 +17860,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="240">
+      <c r="A1" s="241">
         <v>44044</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="241"/>
+      <c r="I1" s="241"/>
+      <c r="J1" s="241"/>
+      <c r="K1" s="241"/>
+      <c r="L1" s="241"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="243" t="s">
+      <c r="A2" s="244" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="243"/>
-      <c r="C2" s="243"/>
-      <c r="D2" s="243"/>
-      <c r="E2" s="243"/>
+      <c r="B2" s="244"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="244"/>
+      <c r="E2" s="244"/>
       <c r="F2" s="88"/>
-      <c r="G2" s="244" t="s">
+      <c r="G2" s="245" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
+      <c r="H2" s="245"/>
+      <c r="I2" s="245"/>
+      <c r="J2" s="245"/>
+      <c r="K2" s="245"/>
+      <c r="L2" s="245"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -18557,6 +18557,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024D76020AE708242B68336FA618CBCDF" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0f8ef3af180fb4ddb5e95743212642f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df3f84f5-0dce-435a-abac-67420900ba59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2069e023351266972e9c1aca68960d8c" ns3:_="">
     <xsd:import namespace="df3f84f5-0dce-435a-abac-67420900ba59"/>
@@ -18726,15 +18735,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11DF5BFB-C4A2-42C5-9ACB-F42BB2AD57D5}">
   <ds:schemaRefs>
@@ -18745,6 +18745,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0955E539-E9CC-455F-B094-E363B2CCC487}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4845A164-C435-4094-8F0C-F88A8D76F182}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18760,12 +18768,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0955E539-E9CC-455F-B094-E363B2CCC487}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>